<commit_message>
Fix voor domein in Exceldatasets
</commit_message>
<xml_diff>
--- a/catalogusdata/Concepten/Regressietest/xls/Datacontrole attributen.xlsx
+++ b/catalogusdata/Concepten/Regressietest/xls/Datacontrole attributen.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24240" windowHeight="13740" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24240" windowHeight="13740"/>
   </bookViews>
   <sheets>
     <sheet name="URI schema" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="124">
   <si>
     <t>tabblad</t>
   </si>
@@ -394,6 +394,9 @@
   </si>
   <si>
     <t>http://xmlns.com/foaf/0.1/{eigenschap}</t>
+  </si>
+  <si>
+    <t>http://data.test.pdok.nl/catalogus/dso/id/concept/{domein}</t>
   </si>
 </sst>
 </file>
@@ -802,10 +805,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E42"/>
+  <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -957,10 +960,10 @@
         <v>69</v>
       </c>
       <c r="B10" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>82</v>
+        <v>123</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -968,10 +971,10 @@
         <v>69</v>
       </c>
       <c r="B11" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -979,10 +982,10 @@
         <v>69</v>
       </c>
       <c r="B12" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -990,10 +993,10 @@
         <v>69</v>
       </c>
       <c r="B13" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -1001,10 +1004,10 @@
         <v>69</v>
       </c>
       <c r="B14" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -1012,24 +1015,21 @@
         <v>69</v>
       </c>
       <c r="B15" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="B16" t="s">
-        <v>65</v>
-      </c>
-      <c r="C16" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1037,60 +1037,60 @@
         <v>64</v>
       </c>
       <c r="B17" t="s">
-        <v>68</v>
+        <v>65</v>
+      </c>
+      <c r="C17" t="s">
+        <v>66</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>79</v>
+        <v>64</v>
       </c>
       <c r="B18" t="s">
-        <v>80</v>
-      </c>
-      <c r="C18" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>79</v>
+        <v>64</v>
       </c>
       <c r="B19" t="s">
-        <v>65</v>
+        <v>27</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>88</v>
+        <v>123</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B20" t="s">
-        <v>33</v>
+        <v>80</v>
       </c>
       <c r="C20" t="s">
-        <v>4</v>
+        <v>66</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B21" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>75</v>
+        <v>88</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -1098,42 +1098,61 @@
         <v>77</v>
       </c>
       <c r="B22" t="s">
-        <v>34</v>
+        <v>33</v>
+      </c>
+      <c r="C22" t="s">
+        <v>4</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>121</v>
+        <v>82</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>117</v>
+        <v>77</v>
       </c>
       <c r="B23" t="s">
-        <v>116</v>
-      </c>
-      <c r="C23" t="s">
-        <v>4</v>
+        <v>74</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>120</v>
+        <v>75</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>77</v>
+      </c>
+      <c r="B24" t="s">
+        <v>34</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>117</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B25" t="s">
+        <v>116</v>
+      </c>
+      <c r="C25" t="s">
+        <v>4</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>117</v>
+      </c>
+      <c r="B26" t="s">
         <v>68</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="D26" s="2" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D25" s="2"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D26" s="2"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D27" s="2"/>
@@ -1182,32 +1201,40 @@
     </row>
     <row r="42" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D42" s="2"/>
+    </row>
+    <row r="43" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D43" s="2"/>
+    </row>
+    <row r="44" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D44" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D5" r:id="rId1"/>
     <hyperlink ref="D6" r:id="rId2" location="{eigenschap}"/>
-    <hyperlink ref="D11" r:id="rId3" display="http://localhost:8080/catalogus/dsoprogramma/id/begrip/{specialisatie}"/>
-    <hyperlink ref="D12" r:id="rId4" display="http://localhost:8080/catalogus/dsoprogramma/id/begrip/{generalisatie}"/>
-    <hyperlink ref="D13" r:id="rId5" display="http://localhost:8080/catalogus/dsoprogramma/id/begrip/{onderdeel}"/>
-    <hyperlink ref="D14" r:id="rId6" display="http://localhost:8080/catalogus/dsoprogramma/id/begrip/{bestaatuit}"/>
-    <hyperlink ref="D15" r:id="rId7" display="http://localhost:8080/catalogus/dsoprogramma/id/begrip/{betrekkingop}"/>
-    <hyperlink ref="D16" r:id="rId8" display="http://localhost:8080/catalogus/dso/id/collection/{collectie}"/>
-    <hyperlink ref="D17" r:id="rId9" display="http://localhost:8080/dsoprogramma/id/begrip/{begrip}"/>
+    <hyperlink ref="D12" r:id="rId3" display="http://localhost:8080/catalogus/dsoprogramma/id/begrip/{specialisatie}"/>
+    <hyperlink ref="D13" r:id="rId4" display="http://localhost:8080/catalogus/dsoprogramma/id/begrip/{generalisatie}"/>
+    <hyperlink ref="D14" r:id="rId5" display="http://localhost:8080/catalogus/dsoprogramma/id/begrip/{onderdeel}"/>
+    <hyperlink ref="D15" r:id="rId6" display="http://localhost:8080/catalogus/dsoprogramma/id/begrip/{bestaatuit}"/>
+    <hyperlink ref="D16" r:id="rId7" display="http://localhost:8080/catalogus/dsoprogramma/id/begrip/{betrekkingop}"/>
+    <hyperlink ref="D17" r:id="rId8" display="http://localhost:8080/catalogus/dso/id/collection/{collectie}"/>
+    <hyperlink ref="D18" r:id="rId9" display="http://localhost:8080/dsoprogramma/id/begrip/{begrip}"/>
     <hyperlink ref="D9" r:id="rId10" display="http://localhost:8080/dsoprogramma/id/begrip/{begrip}"/>
     <hyperlink ref="D7" r:id="rId11" location="{eigenschap}"/>
     <hyperlink ref="D2" r:id="rId12" location="{klasse}"/>
-    <hyperlink ref="D10" r:id="rId13" display="http://localhost:8080/catalogus/dso/id/concept/{bron}"/>
-    <hyperlink ref="D21" r:id="rId14"/>
-    <hyperlink ref="D20" r:id="rId15" display="http://localhost:8080/catalogus/dso/id/concept/{bron}"/>
-    <hyperlink ref="D18" r:id="rId16" display="http://localhost:8080/catalogus/dso/id/collection/{waardelijst}"/>
-    <hyperlink ref="D19" r:id="rId17" display="http://localhost:8080/catalogus/dso/id/collection/{collectie}"/>
-    <hyperlink ref="D23" r:id="rId18"/>
-    <hyperlink ref="D24" r:id="rId19" display="http://localhost:8080/dsoprogramma/id/begrip/{begrip}"/>
+    <hyperlink ref="D11" r:id="rId13" display="http://localhost:8080/catalogus/dso/id/concept/{bron}"/>
+    <hyperlink ref="D23" r:id="rId14"/>
+    <hyperlink ref="D22" r:id="rId15" display="http://localhost:8080/catalogus/dso/id/concept/{bron}"/>
+    <hyperlink ref="D20" r:id="rId16" display="http://localhost:8080/catalogus/dso/id/collection/{waardelijst}"/>
+    <hyperlink ref="D21" r:id="rId17" display="http://localhost:8080/catalogus/dso/id/collection/{collectie}"/>
+    <hyperlink ref="D25" r:id="rId18"/>
+    <hyperlink ref="D26" r:id="rId19" display="http://localhost:8080/dsoprogramma/id/begrip/{begrip}"/>
     <hyperlink ref="D8" r:id="rId20"/>
+    <hyperlink ref="D10" r:id="rId21"/>
+    <hyperlink ref="D19" r:id="rId22"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId21"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId23"/>
 </worksheet>
 </file>
 
@@ -2476,7 +2503,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:F2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fix voor relaties Excelbestanden
</commit_message>
<xml_diff>
--- a/catalogusdata/Concepten/Regressietest/xls/Datacontrole attributen.xlsx
+++ b/catalogusdata/Concepten/Regressietest/xls/Datacontrole attributen.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="129">
   <si>
     <t>tabblad</t>
   </si>
@@ -397,6 +397,21 @@
   </si>
   <si>
     <t>http://data.test.pdok.nl/catalogus/dso/id/concept/{domein}</t>
+  </si>
+  <si>
+    <t>http://data.test.pdok.nl/catalogus/dso/id/concept/{focus}</t>
+  </si>
+  <si>
+    <t>http://data.test.pdok.nl/catalogus/dso/id/concept/{hetzelfde}</t>
+  </si>
+  <si>
+    <t>http://data.test.pdok.nl/catalogus/dso/id/concept/{gerelateerd}</t>
+  </si>
+  <si>
+    <t>http://data.test.pdok.nl/catalogus/dso/id/concept/{brederdan}</t>
+  </si>
+  <si>
+    <t>http://data.test.pdok.nl/catalogus/dso/id/concept/{engerdan}</t>
   </si>
 </sst>
 </file>
@@ -805,10 +820,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E44"/>
+  <dimension ref="A1:E49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1034,140 +1049,180 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="B17" t="s">
-        <v>65</v>
-      </c>
-      <c r="C17" t="s">
-        <v>66</v>
+        <v>101</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>88</v>
+        <v>124</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="B18" t="s">
-        <v>68</v>
+        <v>104</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>81</v>
+        <v>125</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="B19" t="s">
-        <v>27</v>
+        <v>107</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="B20" t="s">
-        <v>80</v>
-      </c>
-      <c r="C20" t="s">
-        <v>66</v>
+        <v>110</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>89</v>
+        <v>127</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="B21" t="s">
-        <v>65</v>
+        <v>113</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>88</v>
+        <v>128</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="B22" t="s">
-        <v>33</v>
+        <v>65</v>
       </c>
       <c r="C22" t="s">
-        <v>4</v>
+        <v>66</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="B23" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="B24" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>117</v>
+        <v>79</v>
       </c>
       <c r="B25" t="s">
-        <v>116</v>
+        <v>80</v>
       </c>
       <c r="C25" t="s">
-        <v>4</v>
+        <v>66</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>120</v>
+        <v>89</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>79</v>
+      </c>
+      <c r="B26" t="s">
+        <v>65</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>77</v>
+      </c>
+      <c r="B27" t="s">
+        <v>33</v>
+      </c>
+      <c r="C27" t="s">
+        <v>4</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>77</v>
+      </c>
+      <c r="B28" t="s">
+        <v>74</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>77</v>
+      </c>
+      <c r="B29" t="s">
+        <v>34</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>117</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B30" t="s">
+        <v>116</v>
+      </c>
+      <c r="C30" t="s">
+        <v>4</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>117</v>
+      </c>
+      <c r="B31" t="s">
         <v>68</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="D31" s="2" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D27" s="2"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D28" s="2"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D29" s="2"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D30" s="2"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D31" s="2"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D32" s="2"/>
@@ -1207,6 +1262,21 @@
     </row>
     <row r="44" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D44" s="2"/>
+    </row>
+    <row r="45" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D45" s="2"/>
+    </row>
+    <row r="46" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D46" s="2"/>
+    </row>
+    <row r="47" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D47" s="2"/>
+    </row>
+    <row r="48" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D48" s="2"/>
+    </row>
+    <row r="49" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D49" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1217,24 +1287,29 @@
     <hyperlink ref="D14" r:id="rId5" display="http://localhost:8080/catalogus/dsoprogramma/id/begrip/{onderdeel}"/>
     <hyperlink ref="D15" r:id="rId6" display="http://localhost:8080/catalogus/dsoprogramma/id/begrip/{bestaatuit}"/>
     <hyperlink ref="D16" r:id="rId7" display="http://localhost:8080/catalogus/dsoprogramma/id/begrip/{betrekkingop}"/>
-    <hyperlink ref="D17" r:id="rId8" display="http://localhost:8080/catalogus/dso/id/collection/{collectie}"/>
-    <hyperlink ref="D18" r:id="rId9" display="http://localhost:8080/dsoprogramma/id/begrip/{begrip}"/>
+    <hyperlink ref="D22" r:id="rId8" display="http://localhost:8080/catalogus/dso/id/collection/{collectie}"/>
+    <hyperlink ref="D23" r:id="rId9" display="http://localhost:8080/dsoprogramma/id/begrip/{begrip}"/>
     <hyperlink ref="D9" r:id="rId10" display="http://localhost:8080/dsoprogramma/id/begrip/{begrip}"/>
     <hyperlink ref="D7" r:id="rId11" location="{eigenschap}"/>
     <hyperlink ref="D2" r:id="rId12" location="{klasse}"/>
     <hyperlink ref="D11" r:id="rId13" display="http://localhost:8080/catalogus/dso/id/concept/{bron}"/>
-    <hyperlink ref="D23" r:id="rId14"/>
-    <hyperlink ref="D22" r:id="rId15" display="http://localhost:8080/catalogus/dso/id/concept/{bron}"/>
-    <hyperlink ref="D20" r:id="rId16" display="http://localhost:8080/catalogus/dso/id/collection/{waardelijst}"/>
-    <hyperlink ref="D21" r:id="rId17" display="http://localhost:8080/catalogus/dso/id/collection/{collectie}"/>
-    <hyperlink ref="D25" r:id="rId18"/>
-    <hyperlink ref="D26" r:id="rId19" display="http://localhost:8080/dsoprogramma/id/begrip/{begrip}"/>
+    <hyperlink ref="D28" r:id="rId14"/>
+    <hyperlink ref="D27" r:id="rId15" display="http://localhost:8080/catalogus/dso/id/concept/{bron}"/>
+    <hyperlink ref="D25" r:id="rId16" display="http://localhost:8080/catalogus/dso/id/collection/{waardelijst}"/>
+    <hyperlink ref="D26" r:id="rId17" display="http://localhost:8080/catalogus/dso/id/collection/{collectie}"/>
+    <hyperlink ref="D30" r:id="rId18"/>
+    <hyperlink ref="D31" r:id="rId19" display="http://localhost:8080/dsoprogramma/id/begrip/{begrip}"/>
     <hyperlink ref="D8" r:id="rId20"/>
     <hyperlink ref="D10" r:id="rId21"/>
-    <hyperlink ref="D19" r:id="rId22"/>
+    <hyperlink ref="D24" r:id="rId22"/>
+    <hyperlink ref="D17" r:id="rId23"/>
+    <hyperlink ref="D18" r:id="rId24"/>
+    <hyperlink ref="D19" r:id="rId25"/>
+    <hyperlink ref="D20" r:id="rId26"/>
+    <hyperlink ref="D21" r:id="rId27"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId23"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId28"/>
 </worksheet>
 </file>
 

</xml_diff>